<commit_message>
Updated for later versions of EA
Updated for later versions of EA
</commit_message>
<xml_diff>
--- a/Technical Files/MS Access Queries for BRIDG/EAP Script - Validate BRIDG Model - Documentation.xlsx
+++ b/Technical Files/MS Access Queries for BRIDG/EAP Script - Validate BRIDG Model - Documentation.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wverhoef\Documents\BRIDG\BRIDG R5.1\SVN to GitHub Transition\bridg-model\Technical Files\MS Access Queries for BRIDG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wverhoef\Documents\BRIDG\BRIDG R5.1\Release Prep - BRIDG 5.0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1095,9 +1095,6 @@
     <t>Open the BRIDG file to be validated in Enterprise Architect</t>
   </si>
   <si>
-    <t>In the "Find Command" field on menu bar, enter "Scripting" and hit Return (opens scripting window)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Expand “Local Scripts” </t>
   </si>
   <si>
@@ -1126,6 +1123,9 @@
   </si>
   <si>
     <t>FYI:  Some messages listed as Error may actually be OK to ignore, for instance the color coding validation is not working properly on the Biospecimen Sub-Domain.</t>
+  </si>
+  <si>
+    <t>In the "Find Command" field on menu bar, enter "Scripting" and hit Return (opens scripting window) or from the main menu select Tools &gt; Scripting</t>
   </si>
 </sst>
 </file>
@@ -1608,10 +1608,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,12 +1627,12 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1641,48 +1642,48 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="18" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="18" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="18" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="18" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C13" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -1694,10 +1695,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -2950,6 +2952,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3777,6 +3780,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>